<commit_message>
Feature : Tournament deck breakdown - update hash csv - update meta archetype - new module stat_helper
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/FortuneHandMeta.xlsx
+++ b/Excel_and_CSV/FortuneHandMeta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Default_WS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Bitbucket_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CCC9E2-DC33-4E55-896D-CA9ABA2B22D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1C9518-10DE-4858-94CD-6990416C01CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7AF58FAE-3130-444B-A793-BB4BE2D0A20F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7AF58FAE-3130-444B-A793-BB4BE2D0A20F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="138">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Pure Terror Forest</t>
   </si>
   <si>
-    <t>Roach-Terror Forest</t>
-  </si>
-  <si>
-    <t>Pure Roach Forest</t>
-  </si>
-  <si>
     <t>Evo Forest</t>
   </si>
   <si>
@@ -135,12 +129,6 @@
     <t>XII. Zelgenea, The World</t>
   </si>
   <si>
-    <t>Luxblade Arriet</t>
-  </si>
-  <si>
-    <t>6td16</t>
-  </si>
-  <si>
     <t>Stroke of Conviction</t>
   </si>
   <si>
@@ -309,9 +297,6 @@
     <t>Wrath Blood</t>
   </si>
   <si>
-    <t>Garnet Waltz</t>
-  </si>
-  <si>
     <t>Permafrost Behemoth</t>
   </si>
   <si>
@@ -324,18 +309,12 @@
     <t>Creeping Madness</t>
   </si>
   <si>
-    <t>6yx6Q</t>
-  </si>
-  <si>
     <t>Haven</t>
   </si>
   <si>
     <t>Elana Haven</t>
   </si>
   <si>
-    <t>Amulet Haven</t>
-  </si>
-  <si>
     <t>Portal</t>
   </si>
   <si>
@@ -390,12 +369,6 @@
     <t>6vvVo</t>
   </si>
   <si>
-    <t>Calm Featherfolk</t>
-  </si>
-  <si>
-    <t>6vPmi</t>
-  </si>
-  <si>
     <t>6s5My</t>
   </si>
   <si>
@@ -408,18 +381,12 @@
     <t>6-UTy</t>
   </si>
   <si>
-    <t>Fieran, Havensent Wind God</t>
-  </si>
-  <si>
     <t>6td0o</t>
   </si>
   <si>
     <t>Kagemitsu, Matchless Blade</t>
   </si>
   <si>
-    <t>Jerva Dragon</t>
-  </si>
-  <si>
     <t>Jerva, Wyrm Transcendent</t>
   </si>
   <si>
@@ -441,16 +408,43 @@
     <t>Phantasmal Fairy Dragon</t>
   </si>
   <si>
-    <t>6-Ntw</t>
-  </si>
-  <si>
-    <t>Sudden Shower</t>
-  </si>
-  <si>
     <t>gXuCg</t>
   </si>
   <si>
     <t>gZ1SK</t>
+  </si>
+  <si>
+    <t>6-SmQ</t>
+  </si>
+  <si>
+    <t>Resolve of the Fallen</t>
+  </si>
+  <si>
+    <t>Roach Accel Forest</t>
+  </si>
+  <si>
+    <t>Jerva/Evo Dragon</t>
+  </si>
+  <si>
+    <t>6yypo</t>
+  </si>
+  <si>
+    <t>Nerea, Beast Empress</t>
+  </si>
+  <si>
+    <t>VIII. Sofina, Strength</t>
+  </si>
+  <si>
+    <t>719NI</t>
+  </si>
+  <si>
+    <t>Sofina/Amulet Haven</t>
+  </si>
+  <si>
+    <t>Roach Natura Forest</t>
+  </si>
+  <si>
+    <t>Ernesta, Weapons Hawker</t>
   </si>
 </sst>
 </file>
@@ -804,15 +798,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F378CFE-8D14-43F7-BAF4-3D4A0611FC8D}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
@@ -828,22 +822,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -851,25 +845,25 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -877,727 +871,727 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F6" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
-      </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" t="s">
-        <v>61</v>
-      </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
         <v>59</v>
       </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>63</v>
-      </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="E15" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="F15" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
-      </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" t="s">
         <v>74</v>
       </c>
-      <c r="B17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" t="s">
-        <v>78</v>
-      </c>
       <c r="F17" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" t="s">
         <v>74</v>
       </c>
-      <c r="B18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" t="s">
-        <v>78</v>
-      </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
         <v>75</v>
       </c>
-      <c r="B19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" t="s">
-        <v>79</v>
-      </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
         <v>76</v>
       </c>
-      <c r="B20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
         <v>80</v>
       </c>
-      <c r="D20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" t="s">
-        <v>84</v>
-      </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" t="s">
         <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" t="s">
         <v>91</v>
       </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" t="s">
-        <v>96</v>
-      </c>
       <c r="F22" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G22" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="H22" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E23" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
         <v>99</v>
       </c>
-      <c r="B24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" t="s">
-        <v>106</v>
-      </c>
       <c r="D24" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F24" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="D25" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="E25" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F25" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" t="s">
         <v>101</v>
       </c>
-      <c r="C26" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" t="s">
-        <v>108</v>
-      </c>
       <c r="F26" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" t="s">
         <v>101</v>
       </c>
-      <c r="C27" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" t="s">
-        <v>139</v>
-      </c>
-      <c r="E27" t="s">
-        <v>108</v>
-      </c>
       <c r="F27" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" t="s">
         <v>109</v>
       </c>
-      <c r="D28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" t="s">
-        <v>112</v>
-      </c>
-      <c r="F28" t="s">
-        <v>116</v>
-      </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" t="s">
         <v>110</v>
       </c>
-      <c r="D29" t="s">
-        <v>117</v>
-      </c>
       <c r="E29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" t="s">
         <v>110</v>
       </c>
-      <c r="F29" t="s">
-        <v>117</v>
-      </c>
       <c r="G29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
         <v>104</v>
       </c>
-      <c r="B30" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>111</v>
       </c>
-      <c r="D30" t="s">
-        <v>118</v>
-      </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature : Add additional cards in hash
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/FortuneHandMeta.xlsx
+++ b/Excel_and_CSV/FortuneHandMeta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Bitbucket_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1C9518-10DE-4858-94CD-6990416C01CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDEE690-6D9B-4C50-BC29-B4C71597A1F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7AF58FAE-3130-444B-A793-BB4BE2D0A20F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="140">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -378,9 +378,6 @@
     <t>71TeA</t>
   </si>
   <si>
-    <t>6-UTy</t>
-  </si>
-  <si>
     <t>6td0o</t>
   </si>
   <si>
@@ -423,9 +420,6 @@
     <t>Roach Accel Forest</t>
   </si>
   <si>
-    <t>Jerva/Evo Dragon</t>
-  </si>
-  <si>
     <t>6yypo</t>
   </si>
   <si>
@@ -438,13 +432,25 @@
     <t>719NI</t>
   </si>
   <si>
-    <t>Sofina/Amulet Haven</t>
-  </si>
-  <si>
     <t>Roach Natura Forest</t>
   </si>
   <si>
     <t>Ernesta, Weapons Hawker</t>
+  </si>
+  <si>
+    <t>6_AQS</t>
+  </si>
+  <si>
+    <t>Diamond Paladin</t>
+  </si>
+  <si>
+    <t>6_FIy</t>
+  </si>
+  <si>
+    <t>Jerva Evo Dragon</t>
+  </si>
+  <si>
+    <t>Sofina Amulet Haven</t>
   </si>
 </sst>
 </file>
@@ -798,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F378CFE-8D14-43F7-BAF4-3D4A0611FC8D}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,16 +900,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -920,7 +926,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -958,10 +964,10 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
@@ -978,10 +984,10 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -990,10 +996,10 @@
         <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1010,10 +1016,10 @@
         <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -1180,22 +1186,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
         <v>53</v>
       </c>
       <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" t="s">
         <v>118</v>
       </c>
-      <c r="D15" t="s">
-        <v>119</v>
-      </c>
       <c r="E15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" t="s">
         <v>118</v>
-      </c>
-      <c r="F15" t="s">
-        <v>119</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
@@ -1247,7 +1253,7 @@
         <v>74</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G17" t="s">
         <v>19</v>
@@ -1348,10 +1354,10 @@
         <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G21" t="s">
         <v>88</v>
@@ -1380,30 +1386,30 @@
         <v>90</v>
       </c>
       <c r="G22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
         <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" t="s">
         <v>121</v>
       </c>
-      <c r="E23" t="s">
-        <v>122</v>
-      </c>
       <c r="F23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G23" t="s">
         <v>19</v>
@@ -1440,16 +1446,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B25" t="s">
         <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E25" t="s">
         <v>106</v>
@@ -1501,7 +1507,7 @@
         <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E27" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Fortune Hand Mini Expac Update
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/FortuneHandMeta.xlsx
+++ b/Excel_and_CSV/FortuneHandMeta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Bitbucket_SV\Excel_and_CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDEE690-6D9B-4C50-BC29-B4C71597A1F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AC4E94-7ED0-44AD-B749-7B253F60138B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7AF58FAE-3130-444B-A793-BB4BE2D0A20F}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="20385" windowHeight="10620" xr2:uid="{7AF58FAE-3130-444B-A793-BB4BE2D0A20F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="148">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -303,12 +297,6 @@
     <t>6v8h6</t>
   </si>
   <si>
-    <t>6v6zQ</t>
-  </si>
-  <si>
-    <t>Creeping Madness</t>
-  </si>
-  <si>
     <t>Haven</t>
   </si>
   <si>
@@ -390,15 +378,6 @@
     <t>6yB_6</t>
   </si>
   <si>
-    <t>Spider Blood</t>
-  </si>
-  <si>
-    <t>6yyq6</t>
-  </si>
-  <si>
-    <t>Ruinweb Spider</t>
-  </si>
-  <si>
     <t>6tEcc</t>
   </si>
   <si>
@@ -451,6 +430,45 @@
   </si>
   <si>
     <t>Sofina Amulet Haven</t>
+  </si>
+  <si>
+    <t>Corruption Blood</t>
+  </si>
+  <si>
+    <t>Baal</t>
+  </si>
+  <si>
+    <t>70mz6</t>
+  </si>
+  <si>
+    <t>6ywNi</t>
+  </si>
+  <si>
+    <t>Ravening Corruption</t>
+  </si>
+  <si>
+    <t>Contemptous Demon</t>
+  </si>
+  <si>
+    <t>70kWi</t>
+  </si>
+  <si>
+    <t>Ra Haven</t>
+  </si>
+  <si>
+    <t>719Nc</t>
+  </si>
+  <si>
+    <t>Ra, Radiance Incarnate</t>
+  </si>
+  <si>
+    <t>Nepthys Shadow</t>
+  </si>
+  <si>
+    <t>Nephthys, Goddess of Amenta</t>
+  </si>
+  <si>
+    <t>70OYc</t>
   </si>
 </sst>
 </file>
@@ -802,19 +820,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F378CFE-8D14-43F7-BAF4-3D4A0611FC8D}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
@@ -900,16 +918,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -926,7 +944,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -964,10 +982,10 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
@@ -984,10 +1002,10 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -996,10 +1014,10 @@
         <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1016,10 +1034,10 @@
         <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -1186,22 +1204,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
         <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
@@ -1238,22 +1256,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
         <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>146</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="F17" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="G17" t="s">
         <v>19</v>
@@ -1279,7 +1297,7 @@
         <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="G18" t="s">
         <v>19</v>
@@ -1290,22 +1308,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
         <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
@@ -1316,22 +1334,22 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
         <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
         <v>19</v>
@@ -1342,100 +1360,100 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
         <v>85</v>
       </c>
       <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" t="s">
         <v>88</v>
       </c>
-      <c r="D22" t="s">
+      <c r="H22" t="s">
         <v>89</v>
-      </c>
-      <c r="E22" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" t="s">
-        <v>121</v>
-      </c>
-      <c r="H22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B23" t="s">
         <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="D23" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="E23" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="F23" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="H23" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="F24" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="G24" t="s">
         <v>19</v>
@@ -1446,22 +1464,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="E25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" t="s">
         <v>106</v>
-      </c>
-      <c r="F25" t="s">
-        <v>107</v>
       </c>
       <c r="G25" t="s">
         <v>19</v>
@@ -1472,22 +1490,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>144</v>
       </c>
       <c r="D26" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="F26" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="G26" t="s">
         <v>19</v>
@@ -1498,22 +1516,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F27" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G27" t="s">
         <v>19</v>
@@ -1524,22 +1542,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E28" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G28" t="s">
         <v>19</v>
@@ -1550,19 +1568,19 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
         <v>98</v>
       </c>
-      <c r="B29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" t="s">
-        <v>103</v>
-      </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F29" t="s">
         <v>110</v>
@@ -1576,31 +1594,84 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D30" t="s">
         <v>111</v>
       </c>
       <c r="E30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" t="s">
+        <v>107</v>
+      </c>
+      <c r="G30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" t="s">
         <v>31</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F32" t="s">
         <v>30</v>
       </c>
-      <c r="G30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="G32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feature : - combine view and stats for ez export - fortune hand meta update
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/FortuneHandMeta.xlsx
+++ b/Excel_and_CSV/FortuneHandMeta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AC4E94-7ED0-44AD-B749-7B253F60138B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5A00EB-5B33-49B9-81AE-9C56B189B712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="20385" windowHeight="10620" xr2:uid="{7AF58FAE-3130-444B-A793-BB4BE2D0A20F}"/>
+    <workbookView xWindow="15" yWindow="165" windowWidth="20385" windowHeight="10620" xr2:uid="{7AF58FAE-3130-444B-A793-BB4BE2D0A20F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -111,24 +111,12 @@
     <t>Sword</t>
   </si>
   <si>
-    <t>Aggro Rally Sword</t>
-  </si>
-  <si>
-    <t>Evo Sword</t>
-  </si>
-  <si>
     <t>6-UTo</t>
   </si>
   <si>
     <t>XII. Zelgenea, The World</t>
   </si>
   <si>
-    <t>Stroke of Conviction</t>
-  </si>
-  <si>
-    <t>6xPSQ</t>
-  </si>
-  <si>
     <t>Rune</t>
   </si>
   <si>
@@ -165,12 +153,6 @@
     <t>Arcane Item Shop</t>
   </si>
   <si>
-    <t>Kyoka, Prize Pupil</t>
-  </si>
-  <si>
-    <t>6ty_2</t>
-  </si>
-  <si>
     <t>Kuon, Founder of Onmyodo</t>
   </si>
   <si>
@@ -414,18 +396,6 @@
     <t>Roach Natura Forest</t>
   </si>
   <si>
-    <t>Ernesta, Weapons Hawker</t>
-  </si>
-  <si>
-    <t>6_AQS</t>
-  </si>
-  <si>
-    <t>Diamond Paladin</t>
-  </si>
-  <si>
-    <t>6_FIy</t>
-  </si>
-  <si>
     <t>Jerva Evo Dragon</t>
   </si>
   <si>
@@ -453,7 +423,76 @@
     <t>70kWi</t>
   </si>
   <si>
-    <t>Ra Haven</t>
+    <t>Nepthys Shadow</t>
+  </si>
+  <si>
+    <t>Nephthys, Goddess of Amenta</t>
+  </si>
+  <si>
+    <t>70OYc</t>
+  </si>
+  <si>
+    <t>Whale Dragon</t>
+  </si>
+  <si>
+    <t>Eternal Whale</t>
+  </si>
+  <si>
+    <t>6_zhi</t>
+  </si>
+  <si>
+    <t>Slaughtering Dragonewt</t>
+  </si>
+  <si>
+    <t>6_zhY</t>
+  </si>
+  <si>
+    <t>Satan Haven</t>
+  </si>
+  <si>
+    <t>Temple of Heresy</t>
+  </si>
+  <si>
+    <t>Anomaly Forest</t>
+  </si>
+  <si>
+    <t>Wellspring Elf Princess</t>
+  </si>
+  <si>
+    <t>6lXRo</t>
+  </si>
+  <si>
+    <t>Life Banquet</t>
+  </si>
+  <si>
+    <t>6-rAw</t>
+  </si>
+  <si>
+    <t>Runie, Resolute Diviner</t>
+  </si>
+  <si>
+    <t>6_djc</t>
+  </si>
+  <si>
+    <t>Midrange Shadow</t>
+  </si>
+  <si>
+    <t>6ujqC</t>
+  </si>
+  <si>
+    <t>6umGI</t>
+  </si>
+  <si>
+    <t>Ginsetsu, Great Fox</t>
+  </si>
+  <si>
+    <t>Shuten-Doji</t>
+  </si>
+  <si>
+    <t>Midrange Sword</t>
+  </si>
+  <si>
+    <t>Ra Control Haven</t>
   </si>
   <si>
     <t>719Nc</t>
@@ -462,13 +501,16 @@
     <t>Ra, Radiance Incarnate</t>
   </si>
   <si>
-    <t>Nepthys Shadow</t>
-  </si>
-  <si>
-    <t>Nephthys, Goddess of Amenta</t>
-  </si>
-  <si>
-    <t>70OYc</t>
+    <t>Ward Haven</t>
+  </si>
+  <si>
+    <t>Wilbert, Grand Knight</t>
+  </si>
+  <si>
+    <t>6vX5I</t>
+  </si>
+  <si>
+    <t>717QI</t>
   </si>
 </sst>
 </file>
@@ -820,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F378CFE-8D14-43F7-BAF4-3D4A0611FC8D}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,22 +908,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -892,22 +934,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -918,74 +960,74 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
@@ -996,48 +1038,48 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>132</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -1048,48 +1090,48 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
         <v>40</v>
-      </c>
-      <c r="H9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
       <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
         <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>51</v>
       </c>
       <c r="G10" t="s">
         <v>19</v>
@@ -1100,22 +1142,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
         <v>19</v>
@@ -1126,48 +1168,48 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>50</v>
-      </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>139</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
@@ -1178,22 +1220,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
         <v>58</v>
       </c>
-      <c r="D14" t="s">
-        <v>66</v>
-      </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
@@ -1204,22 +1246,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" t="s">
-        <v>115</v>
-      </c>
       <c r="F15" t="s">
-        <v>116</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
@@ -1230,22 +1272,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="G16" t="s">
         <v>19</v>
@@ -1256,22 +1298,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="G17" t="s">
         <v>19</v>
@@ -1282,22 +1324,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="F18" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="G18" t="s">
         <v>19</v>
@@ -1308,22 +1350,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
@@ -1334,22 +1376,22 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" t="s">
         <v>77</v>
-      </c>
-      <c r="F20" t="s">
-        <v>78</v>
       </c>
       <c r="G20" t="s">
         <v>19</v>
@@ -1360,22 +1402,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" t="s">
         <v>72</v>
-      </c>
-      <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" t="s">
-        <v>81</v>
       </c>
       <c r="G21" t="s">
         <v>19</v>
@@ -1386,77 +1428,77 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>149</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>153</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="F22" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="G22" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="H22" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>136</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="G23" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="G24" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="H24" t="s">
         <v>19</v>
@@ -1464,25 +1506,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="F25" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="H25" t="s">
         <v>19</v>
@@ -1490,22 +1532,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F26" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="G26" t="s">
         <v>19</v>
@@ -1516,22 +1558,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="D27" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="F27" t="s">
-        <v>105</v>
+        <v>161</v>
       </c>
       <c r="G27" t="s">
         <v>19</v>
@@ -1542,22 +1584,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F28" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G28" t="s">
         <v>19</v>
@@ -1568,22 +1610,22 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" t="s">
         <v>98</v>
       </c>
-      <c r="D29" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>99</v>
-      </c>
-      <c r="F29" t="s">
-        <v>110</v>
       </c>
       <c r="G29" t="s">
         <v>19</v>
@@ -1594,22 +1636,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="E30" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="F30" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="G30" t="s">
         <v>19</v>
@@ -1620,22 +1662,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>157</v>
       </c>
       <c r="D31" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="E31" t="s">
-        <v>101</v>
+        <v>157</v>
       </c>
       <c r="F31" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="G31" t="s">
         <v>19</v>
@@ -1646,27 +1688,131 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" t="s">
         <v>95</v>
       </c>
-      <c r="B32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D35" t="s">
         <v>102</v>
       </c>
-      <c r="D32" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="E35" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfix : -excel module convert flexibility - ban peek type casting and dictionary fix - meta changes
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/FortuneHandMeta.xlsx
+++ b/Excel_and_CSV/FortuneHandMeta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE31B943-776D-4319-85D8-67608A83BE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D23988-352E-4A65-B9C6-02CB54D3C0EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="165" windowWidth="20385" windowHeight="10620" xr2:uid="{7AF58FAE-3130-444B-A793-BB4BE2D0A20F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7AF58FAE-3130-444B-A793-BB4BE2D0A20F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -495,9 +495,6 @@
     <t>Yukari, Holy Guardian</t>
   </si>
   <si>
-    <t>Aggro Blood</t>
-  </si>
-  <si>
     <t>Milteo OTK Shadow</t>
   </si>
   <si>
@@ -517,6 +514,9 @@
   </si>
   <si>
     <t>6yAHQ</t>
+  </si>
+  <si>
+    <t>Corruption Blood</t>
   </si>
 </sst>
 </file>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F378CFE-8D14-43F7-BAF4-3D4A0611FC8D}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,22 +1252,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
       <c r="C15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" t="s">
         <v>161</v>
       </c>
-      <c r="D15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>162</v>
-      </c>
-      <c r="F15" t="s">
-        <v>163</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B23" t="s">
         <v>63</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B26" t="s">
         <v>79</v>

</xml_diff>